<commit_message>
create all entity and dto
</commit_message>
<xml_diff>
--- a/Task.xlsx
+++ b/Task.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
   </bookViews>
   <sheets>
     <sheet name="Back-end" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="30">
   <si>
     <t>Num.</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>Homepage Template</t>
+  </si>
+  <si>
+    <t>CRUD all Entity</t>
   </si>
 </sst>
 </file>
@@ -542,30 +545,6 @@
     <xf numFmtId="14" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -576,6 +555,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -888,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,54 +907,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="34"/>
+      <c r="B3" s="26"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="26" t="s">
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="35" t="s">
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="31" t="s">
+      <c r="K5" s="35" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="28"/>
-      <c r="C6" s="30"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
@@ -970,8 +973,8 @@
       <c r="I6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="36"/>
-      <c r="K6" s="32"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="36"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
@@ -1097,7 +1100,9 @@
       <c r="B11" s="5">
         <v>5</v>
       </c>
-      <c r="C11" s="14"/>
+      <c r="C11" s="14" t="s">
+        <v>29</v>
+      </c>
       <c r="D11" s="21"/>
       <c r="E11" s="21"/>
       <c r="F11" s="21"/>
@@ -1421,8 +1426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1437,54 +1442,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="34"/>
+      <c r="B3" s="26"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="26" t="s">
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="35" t="s">
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="31" t="s">
+      <c r="K5" s="35" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="28"/>
-      <c r="C6" s="30"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1503,8 +1508,8 @@
       <c r="I6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="36"/>
-      <c r="K6" s="32"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="36"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="3">

</xml_diff>

<commit_message>
change source structure (dataquery, admin-portal, bookstore-portal)
</commit_message>
<xml_diff>
--- a/Task.xlsx
+++ b/Task.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="35">
   <si>
     <t>Num.</t>
   </si>
@@ -90,9 +90,6 @@
     <t>20/4</t>
   </si>
   <si>
-    <t>CRUD User &amp; Role entity</t>
-  </si>
-  <si>
     <t>Security Configuration</t>
   </si>
   <si>
@@ -114,7 +111,25 @@
     <t>Homepage Template</t>
   </si>
   <si>
-    <t>CRUD all Entity</t>
+    <t>Create User &amp; Role entity</t>
+  </si>
+  <si>
+    <t>Create all Entities</t>
+  </si>
+  <si>
+    <t>8h</t>
+  </si>
+  <si>
+    <t>24/4</t>
+  </si>
+  <si>
+    <t>3 part: dataquery, admin, bookstore</t>
+  </si>
+  <si>
+    <t>6h</t>
+  </si>
+  <si>
+    <t>Change source structure</t>
   </si>
 </sst>
 </file>
@@ -892,7 +907,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,7 +917,7 @@
     <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
     <col min="5" max="9" width="9.140625" style="1"/>
     <col min="10" max="10" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="37.85546875" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -981,7 +996,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D7" s="19" t="s">
         <v>17</v>
@@ -1011,7 +1026,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8" s="21" t="s">
         <v>18</v>
@@ -1071,7 +1086,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>15</v>
@@ -1080,7 +1095,7 @@
         <v>6</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>15</v>
@@ -1089,7 +1104,7 @@
         <v>6</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J10" s="17" t="s">
         <v>14</v>
@@ -1103,28 +1118,60 @@
       <c r="C11" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="17"/>
+      <c r="D11" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="K11" s="6"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" s="5">
         <v>6</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="6"/>
+      <c r="C12" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="5">
@@ -1516,7 +1563,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="19" t="s">
         <v>15</v>
@@ -1546,7 +1593,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" s="21" t="s">
         <v>17</v>
@@ -1576,7 +1623,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="21" t="s">
         <v>19</v>
@@ -1606,7 +1653,7 @@
         <v>4</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>15</v>
@@ -1615,7 +1662,7 @@
         <v>6</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G10" s="11" t="s">
         <v>15</v>
@@ -1624,7 +1671,7 @@
         <v>6</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J10" s="17" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Update code for BookInfo and DeleteBook
</commit_message>
<xml_diff>
--- a/Task.xlsx
+++ b/Task.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
   </bookViews>
   <sheets>
     <sheet name="Back-end" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="52">
   <si>
     <t>Num.</t>
   </si>
@@ -132,16 +132,55 @@
     <t>Change source structure</t>
   </si>
   <si>
-    <t>AddBook</t>
-  </si>
-  <si>
-    <t>BookList</t>
-  </si>
-  <si>
     <t>26/4</t>
   </si>
   <si>
-    <t>AddBook &amp; Book List</t>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>dataquery</t>
+  </si>
+  <si>
+    <t>admin &amp; bookstore</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>AddBook &amp; BookList</t>
+  </si>
+  <si>
+    <t>27/4</t>
+  </si>
+  <si>
+    <t>admin &amp; dataquery</t>
+  </si>
+  <si>
+    <t>AddBook Template</t>
+  </si>
+  <si>
+    <t>BookList Template</t>
+  </si>
+  <si>
+    <t>3h</t>
+  </si>
+  <si>
+    <t>In-progress</t>
+  </si>
+  <si>
+    <t>Update: in-progress</t>
+  </si>
+  <si>
+    <t>CRUD Book</t>
+  </si>
+  <si>
+    <t>BookInfo Template</t>
+  </si>
+  <si>
+    <t>UpdateBook Template</t>
+  </si>
+  <si>
+    <t>20m</t>
   </si>
 </sst>
 </file>
@@ -173,7 +212,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -234,8 +273,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -494,11 +539,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashed">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="dashed">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -572,6 +697,9 @@
     <xf numFmtId="14" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -606,6 +734,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -918,14 +1070,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="47.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
     <col min="5" max="9" width="9.140625" style="1"/>
     <col min="10" max="10" width="11" style="1" bestFit="1" customWidth="1"/>
@@ -934,78 +1087,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="26"/>
+      <c r="B3" s="27"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="31" t="s">
+      <c r="A5" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="B5" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="30" t="s">
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="27" t="s">
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="35" t="s">
+      <c r="K5" s="36" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="32"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="2" t="s">
+      <c r="A6" s="41"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="28"/>
-      <c r="K6" s="36"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="37"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="3">
+      <c r="A7" s="38">
         <v>1</v>
+      </c>
+      <c r="B7" s="43" t="s">
+        <v>37</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>28</v>
@@ -1034,8 +1194,11 @@
       <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="5">
+      <c r="A8" s="5">
         <v>2</v>
+      </c>
+      <c r="B8" s="44" t="s">
+        <v>38</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>21</v>
@@ -1064,8 +1227,11 @@
       <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="5">
+      <c r="A9" s="5">
         <v>3</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>38</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>2</v>
@@ -1094,8 +1260,11 @@
       <c r="K9" s="6"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="5">
+      <c r="A10" s="5">
         <v>4</v>
+      </c>
+      <c r="B10" s="44" t="s">
+        <v>38</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>23</v>
@@ -1124,8 +1293,11 @@
       <c r="K10" s="6"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="5">
+      <c r="A11" s="5">
         <v>5</v>
+      </c>
+      <c r="B11" s="44" t="s">
+        <v>37</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>29</v>
@@ -1154,9 +1326,10 @@
       <c r="K11" s="6"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="5">
+      <c r="A12" s="5">
         <v>6</v>
       </c>
+      <c r="B12" s="44"/>
       <c r="C12" s="14" t="s">
         <v>34</v>
       </c>
@@ -1186,29 +1359,32 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="5">
+      <c r="A13" s="5">
         <v>7</v>
       </c>
+      <c r="B13" s="44" t="s">
+        <v>42</v>
+      </c>
       <c r="C13" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D13" s="21" t="s">
         <v>18</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>17</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J13" s="17" t="s">
         <v>14</v>
@@ -1216,23 +1392,43 @@
       <c r="K13" s="6"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="5">
+      <c r="A14" s="5">
         <v>8</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
+      <c r="B14" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>41</v>
+      </c>
       <c r="I14" s="11"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="6"/>
+      <c r="J14" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="5">
+      <c r="A15" s="5">
         <v>9</v>
       </c>
+      <c r="B15" s="44"/>
       <c r="C15" s="14"/>
       <c r="D15" s="21"/>
       <c r="E15" s="21"/>
@@ -1244,9 +1440,10 @@
       <c r="K15" s="6"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="5">
+      <c r="A16" s="5">
         <v>10</v>
       </c>
+      <c r="B16" s="44"/>
       <c r="C16" s="14"/>
       <c r="D16" s="21"/>
       <c r="E16" s="21"/>
@@ -1257,10 +1454,11 @@
       <c r="J16" s="17"/>
       <c r="K16" s="6"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="5">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
         <v>11</v>
       </c>
+      <c r="B17" s="44"/>
       <c r="C17" s="14"/>
       <c r="D17" s="21"/>
       <c r="E17" s="21"/>
@@ -1271,10 +1469,11 @@
       <c r="J17" s="17"/>
       <c r="K17" s="6"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="5">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
         <v>12</v>
       </c>
+      <c r="B18" s="44"/>
       <c r="C18" s="14"/>
       <c r="D18" s="21"/>
       <c r="E18" s="21"/>
@@ -1285,10 +1484,11 @@
       <c r="J18" s="17"/>
       <c r="K18" s="6"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="5">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
         <v>13</v>
       </c>
+      <c r="B19" s="44"/>
       <c r="C19" s="14"/>
       <c r="D19" s="21"/>
       <c r="E19" s="21"/>
@@ -1299,10 +1499,11 @@
       <c r="J19" s="17"/>
       <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="5">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
         <v>14</v>
       </c>
+      <c r="B20" s="44"/>
       <c r="C20" s="14"/>
       <c r="D20" s="21"/>
       <c r="E20" s="21"/>
@@ -1313,10 +1514,11 @@
       <c r="J20" s="17"/>
       <c r="K20" s="6"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="5">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
         <v>15</v>
       </c>
+      <c r="B21" s="44"/>
       <c r="C21" s="14"/>
       <c r="D21" s="21"/>
       <c r="E21" s="21"/>
@@ -1327,10 +1529,11 @@
       <c r="J21" s="17"/>
       <c r="K21" s="6"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="5">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
         <v>16</v>
       </c>
+      <c r="B22" s="44"/>
       <c r="C22" s="14"/>
       <c r="D22" s="21"/>
       <c r="E22" s="21"/>
@@ -1341,10 +1544,11 @@
       <c r="J22" s="17"/>
       <c r="K22" s="6"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="5">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
         <v>17</v>
       </c>
+      <c r="B23" s="44"/>
       <c r="C23" s="14"/>
       <c r="D23" s="21"/>
       <c r="E23" s="21"/>
@@ -1355,10 +1559,11 @@
       <c r="J23" s="17"/>
       <c r="K23" s="6"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="5">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
         <v>18</v>
       </c>
+      <c r="B24" s="44"/>
       <c r="C24" s="14"/>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
@@ -1369,10 +1574,11 @@
       <c r="J24" s="17"/>
       <c r="K24" s="6"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="5">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
         <v>19</v>
       </c>
+      <c r="B25" s="44"/>
       <c r="C25" s="14"/>
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>
@@ -1383,10 +1589,11 @@
       <c r="J25" s="17"/>
       <c r="K25" s="6"/>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="5">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
         <v>20</v>
       </c>
+      <c r="B26" s="44"/>
       <c r="C26" s="14"/>
       <c r="D26" s="21"/>
       <c r="E26" s="21"/>
@@ -1397,10 +1604,11 @@
       <c r="J26" s="17"/>
       <c r="K26" s="6"/>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="5">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
         <v>21</v>
       </c>
+      <c r="B27" s="44"/>
       <c r="C27" s="14"/>
       <c r="D27" s="21"/>
       <c r="E27" s="21"/>
@@ -1411,10 +1619,11 @@
       <c r="J27" s="17"/>
       <c r="K27" s="6"/>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="5">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
         <v>22</v>
       </c>
+      <c r="B28" s="44"/>
       <c r="C28" s="14"/>
       <c r="D28" s="21"/>
       <c r="E28" s="21"/>
@@ -1425,10 +1634,11 @@
       <c r="J28" s="17"/>
       <c r="K28" s="6"/>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="5">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
         <v>23</v>
       </c>
+      <c r="B29" s="44"/>
       <c r="C29" s="14"/>
       <c r="D29" s="21"/>
       <c r="E29" s="21"/>
@@ -1439,10 +1649,11 @@
       <c r="J29" s="17"/>
       <c r="K29" s="6"/>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="5">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
         <v>24</v>
       </c>
+      <c r="B30" s="44"/>
       <c r="C30" s="14"/>
       <c r="D30" s="21"/>
       <c r="E30" s="21"/>
@@ -1453,10 +1664,11 @@
       <c r="J30" s="17"/>
       <c r="K30" s="6"/>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="5">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
         <v>25</v>
       </c>
+      <c r="B31" s="44"/>
       <c r="C31" s="14"/>
       <c r="D31" s="21"/>
       <c r="E31" s="21"/>
@@ -1467,10 +1679,11 @@
       <c r="J31" s="17"/>
       <c r="K31" s="6"/>
     </row>
-    <row r="32" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="7">
+    <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="7">
         <v>26</v>
       </c>
+      <c r="B32" s="45"/>
       <c r="C32" s="15"/>
       <c r="D32" s="22"/>
       <c r="E32" s="22"/>
@@ -1482,7 +1695,7 @@
       <c r="K32" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="J5:J6"/>
@@ -1491,6 +1704,7 @@
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="K5:K6"/>
+    <mergeCell ref="A5:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1501,14 +1715,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="47.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
     <col min="5" max="9" width="9.140625" style="1"/>
     <col min="10" max="10" width="11" style="1" bestFit="1" customWidth="1"/>
@@ -1517,54 +1732,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="26"/>
+      <c r="B3" s="27"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="31" t="s">
+      <c r="A5" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="B5" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="30" t="s">
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="27" t="s">
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="35" t="s">
+      <c r="K5" s="36" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="32"/>
-      <c r="C6" s="34"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="35"/>
       <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1583,12 +1802,15 @@
       <c r="I6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="28"/>
-      <c r="K6" s="36"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="37"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="3">
+      <c r="A7" s="3">
         <v>1</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>38</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>25</v>
@@ -1617,8 +1839,11 @@
       <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="5">
+      <c r="A8" s="5">
         <v>2</v>
+      </c>
+      <c r="B8" s="44" t="s">
+        <v>38</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>26</v>
@@ -1647,8 +1872,11 @@
       <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="5">
+      <c r="A9" s="5">
         <v>3</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>38</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>27</v>
@@ -1677,8 +1905,11 @@
       <c r="K9" s="6"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="5">
+      <c r="A10" s="5">
         <v>4</v>
+      </c>
+      <c r="B10" s="44" t="s">
+        <v>38</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>24</v>
@@ -1707,29 +1938,32 @@
       <c r="K10" s="6"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="5">
+      <c r="A11" s="5">
         <v>5</v>
       </c>
+      <c r="B11" s="44" t="s">
+        <v>39</v>
+      </c>
       <c r="C11" s="14" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="D11" s="21" t="s">
         <v>18</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G11" s="11" t="s">
         <v>18</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J11" s="17" t="s">
         <v>14</v>
@@ -1737,29 +1971,32 @@
       <c r="K11" s="6"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="5">
+      <c r="A12" s="5">
         <v>6</v>
       </c>
+      <c r="B12" s="44" t="s">
+        <v>39</v>
+      </c>
       <c r="C12" s="14" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="D12" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>17</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J12" s="17" t="s">
         <v>14</v>
@@ -1767,37 +2004,76 @@
       <c r="K12" s="6"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="5">
+      <c r="A13" s="5">
         <v>7</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="17"/>
+      <c r="B13" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="J13" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="K13" s="6"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="5">
+      <c r="A14" s="5">
         <v>8</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="17"/>
+      <c r="B14" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="J14" s="17" t="s">
+        <v>14</v>
+      </c>
       <c r="K14" s="6"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="5">
+      <c r="A15" s="5">
         <v>9</v>
       </c>
+      <c r="B15" s="44"/>
       <c r="C15" s="14"/>
       <c r="D15" s="21"/>
       <c r="E15" s="21"/>
@@ -1809,9 +2085,10 @@
       <c r="K15" s="6"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="5">
+      <c r="A16" s="5">
         <v>10</v>
       </c>
+      <c r="B16" s="44"/>
       <c r="C16" s="14"/>
       <c r="D16" s="21"/>
       <c r="E16" s="21"/>
@@ -1822,10 +2099,11 @@
       <c r="J16" s="17"/>
       <c r="K16" s="6"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="5">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
         <v>11</v>
       </c>
+      <c r="B17" s="44"/>
       <c r="C17" s="14"/>
       <c r="D17" s="21"/>
       <c r="E17" s="21"/>
@@ -1836,10 +2114,11 @@
       <c r="J17" s="17"/>
       <c r="K17" s="6"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="5">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
         <v>12</v>
       </c>
+      <c r="B18" s="44"/>
       <c r="C18" s="14"/>
       <c r="D18" s="21"/>
       <c r="E18" s="21"/>
@@ -1850,10 +2129,11 @@
       <c r="J18" s="17"/>
       <c r="K18" s="6"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="5">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
         <v>13</v>
       </c>
+      <c r="B19" s="44"/>
       <c r="C19" s="14"/>
       <c r="D19" s="21"/>
       <c r="E19" s="21"/>
@@ -1864,10 +2144,11 @@
       <c r="J19" s="17"/>
       <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="5">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
         <v>14</v>
       </c>
+      <c r="B20" s="44"/>
       <c r="C20" s="14"/>
       <c r="D20" s="21"/>
       <c r="E20" s="21"/>
@@ -1878,10 +2159,11 @@
       <c r="J20" s="17"/>
       <c r="K20" s="6"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="5">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
         <v>15</v>
       </c>
+      <c r="B21" s="44"/>
       <c r="C21" s="14"/>
       <c r="D21" s="21"/>
       <c r="E21" s="21"/>
@@ -1892,10 +2174,11 @@
       <c r="J21" s="17"/>
       <c r="K21" s="6"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="5">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
         <v>16</v>
       </c>
+      <c r="B22" s="44"/>
       <c r="C22" s="14"/>
       <c r="D22" s="21"/>
       <c r="E22" s="21"/>
@@ -1906,10 +2189,11 @@
       <c r="J22" s="17"/>
       <c r="K22" s="6"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="5">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
         <v>17</v>
       </c>
+      <c r="B23" s="44"/>
       <c r="C23" s="14"/>
       <c r="D23" s="21"/>
       <c r="E23" s="21"/>
@@ -1920,10 +2204,11 @@
       <c r="J23" s="17"/>
       <c r="K23" s="6"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="5">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
         <v>18</v>
       </c>
+      <c r="B24" s="44"/>
       <c r="C24" s="14"/>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
@@ -1934,10 +2219,11 @@
       <c r="J24" s="17"/>
       <c r="K24" s="6"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="5">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
         <v>19</v>
       </c>
+      <c r="B25" s="44"/>
       <c r="C25" s="14"/>
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>
@@ -1948,10 +2234,11 @@
       <c r="J25" s="17"/>
       <c r="K25" s="6"/>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="5">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
         <v>20</v>
       </c>
+      <c r="B26" s="44"/>
       <c r="C26" s="14"/>
       <c r="D26" s="21"/>
       <c r="E26" s="21"/>
@@ -1962,10 +2249,11 @@
       <c r="J26" s="17"/>
       <c r="K26" s="6"/>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="5">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
         <v>21</v>
       </c>
+      <c r="B27" s="44"/>
       <c r="C27" s="14"/>
       <c r="D27" s="21"/>
       <c r="E27" s="21"/>
@@ -1976,10 +2264,11 @@
       <c r="J27" s="17"/>
       <c r="K27" s="6"/>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="5">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
         <v>22</v>
       </c>
+      <c r="B28" s="44"/>
       <c r="C28" s="14"/>
       <c r="D28" s="21"/>
       <c r="E28" s="21"/>
@@ -1990,10 +2279,11 @@
       <c r="J28" s="17"/>
       <c r="K28" s="6"/>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="5">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
         <v>23</v>
       </c>
+      <c r="B29" s="44"/>
       <c r="C29" s="14"/>
       <c r="D29" s="21"/>
       <c r="E29" s="21"/>
@@ -2004,10 +2294,11 @@
       <c r="J29" s="17"/>
       <c r="K29" s="6"/>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="5">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
         <v>24</v>
       </c>
+      <c r="B30" s="44"/>
       <c r="C30" s="14"/>
       <c r="D30" s="21"/>
       <c r="E30" s="21"/>
@@ -2018,10 +2309,11 @@
       <c r="J30" s="17"/>
       <c r="K30" s="6"/>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="5">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
         <v>25</v>
       </c>
+      <c r="B31" s="44"/>
       <c r="C31" s="14"/>
       <c r="D31" s="21"/>
       <c r="E31" s="21"/>
@@ -2032,10 +2324,11 @@
       <c r="J31" s="17"/>
       <c r="K31" s="6"/>
     </row>
-    <row r="32" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="7">
+    <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="7">
         <v>26</v>
       </c>
+      <c r="B32" s="45"/>
       <c r="C32" s="15"/>
       <c r="D32" s="22"/>
       <c r="E32" s="22"/>
@@ -2047,7 +2340,7 @@
       <c r="K32" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="B5:B6"/>
@@ -2056,6 +2349,7 @@
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="K5:K6"/>
+    <mergeCell ref="A5:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add code for updateBook
</commit_message>
<xml_diff>
--- a/Task.xlsx
+++ b/Task.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="52">
   <si>
     <t>Num.</t>
   </si>
@@ -162,15 +162,6 @@
     <t>BookList Template</t>
   </si>
   <si>
-    <t>3h</t>
-  </si>
-  <si>
-    <t>In-progress</t>
-  </si>
-  <si>
-    <t>Update: in-progress</t>
-  </si>
-  <si>
     <t>CRUD Book</t>
   </si>
   <si>
@@ -181,6 +172,15 @@
   </si>
   <si>
     <t>20m</t>
+  </si>
+  <si>
+    <t>2/5</t>
+  </si>
+  <si>
+    <t>BookDetail</t>
+  </si>
+  <si>
+    <t>BookShelf</t>
   </si>
 </sst>
 </file>
@@ -623,7 +623,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -700,6 +700,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -718,46 +730,37 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1071,7 +1074,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,58 +1090,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="27"/>
+      <c r="B3" s="31"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="31" t="s">
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="28" t="s">
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="36" t="s">
+      <c r="K5" s="40" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="41"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="35"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="39"/>
       <c r="D6" s="25" t="s">
         <v>3</v>
       </c>
@@ -1157,14 +1160,14 @@
       <c r="I6" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="29"/>
-      <c r="K6" s="37"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="41"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="38">
+      <c r="A7" s="26">
         <v>1</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="27" t="s">
         <v>37</v>
       </c>
       <c r="C7" s="13" t="s">
@@ -1197,7 +1200,7 @@
       <c r="A8" s="5">
         <v>2</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="28" t="s">
         <v>38</v>
       </c>
       <c r="C8" s="14" t="s">
@@ -1230,7 +1233,7 @@
       <c r="A9" s="5">
         <v>3</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="28" t="s">
         <v>38</v>
       </c>
       <c r="C9" s="14" t="s">
@@ -1263,7 +1266,7 @@
       <c r="A10" s="5">
         <v>4</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="28" t="s">
         <v>38</v>
       </c>
       <c r="C10" s="14" t="s">
@@ -1296,7 +1299,7 @@
       <c r="A11" s="5">
         <v>5</v>
       </c>
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="28" t="s">
         <v>37</v>
       </c>
       <c r="C11" s="14" t="s">
@@ -1329,7 +1332,7 @@
       <c r="A12" s="5">
         <v>6</v>
       </c>
-      <c r="B12" s="44"/>
+      <c r="B12" s="28"/>
       <c r="C12" s="14" t="s">
         <v>34</v>
       </c>
@@ -1362,7 +1365,7 @@
       <c r="A13" s="5">
         <v>7</v>
       </c>
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="28" t="s">
         <v>42</v>
       </c>
       <c r="C13" s="14" t="s">
@@ -1395,11 +1398,11 @@
       <c r="A14" s="5">
         <v>8</v>
       </c>
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="28" t="s">
         <v>42</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D14" s="21" t="s">
         <v>15</v>
@@ -1411,25 +1414,27 @@
         <v>41</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="H14" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="I14" s="11"/>
+      <c r="I14" s="46" t="s">
+        <v>49</v>
+      </c>
       <c r="J14" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>47</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="K14" s="6"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>9</v>
       </c>
-      <c r="B15" s="44"/>
-      <c r="C15" s="14"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="14" t="s">
+        <v>51</v>
+      </c>
       <c r="D15" s="21"/>
       <c r="E15" s="21"/>
       <c r="F15" s="21"/>
@@ -1443,8 +1448,10 @@
       <c r="A16" s="5">
         <v>10</v>
       </c>
-      <c r="B16" s="44"/>
-      <c r="C16" s="14"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="14" t="s">
+        <v>50</v>
+      </c>
       <c r="D16" s="21"/>
       <c r="E16" s="21"/>
       <c r="F16" s="21"/>
@@ -1458,7 +1465,7 @@
       <c r="A17" s="5">
         <v>11</v>
       </c>
-      <c r="B17" s="44"/>
+      <c r="B17" s="28"/>
       <c r="C17" s="14"/>
       <c r="D17" s="21"/>
       <c r="E17" s="21"/>
@@ -1473,7 +1480,7 @@
       <c r="A18" s="5">
         <v>12</v>
       </c>
-      <c r="B18" s="44"/>
+      <c r="B18" s="28"/>
       <c r="C18" s="14"/>
       <c r="D18" s="21"/>
       <c r="E18" s="21"/>
@@ -1488,7 +1495,7 @@
       <c r="A19" s="5">
         <v>13</v>
       </c>
-      <c r="B19" s="44"/>
+      <c r="B19" s="28"/>
       <c r="C19" s="14"/>
       <c r="D19" s="21"/>
       <c r="E19" s="21"/>
@@ -1503,7 +1510,7 @@
       <c r="A20" s="5">
         <v>14</v>
       </c>
-      <c r="B20" s="44"/>
+      <c r="B20" s="28"/>
       <c r="C20" s="14"/>
       <c r="D20" s="21"/>
       <c r="E20" s="21"/>
@@ -1518,7 +1525,7 @@
       <c r="A21" s="5">
         <v>15</v>
       </c>
-      <c r="B21" s="44"/>
+      <c r="B21" s="28"/>
       <c r="C21" s="14"/>
       <c r="D21" s="21"/>
       <c r="E21" s="21"/>
@@ -1533,7 +1540,7 @@
       <c r="A22" s="5">
         <v>16</v>
       </c>
-      <c r="B22" s="44"/>
+      <c r="B22" s="28"/>
       <c r="C22" s="14"/>
       <c r="D22" s="21"/>
       <c r="E22" s="21"/>
@@ -1548,7 +1555,7 @@
       <c r="A23" s="5">
         <v>17</v>
       </c>
-      <c r="B23" s="44"/>
+      <c r="B23" s="28"/>
       <c r="C23" s="14"/>
       <c r="D23" s="21"/>
       <c r="E23" s="21"/>
@@ -1563,7 +1570,7 @@
       <c r="A24" s="5">
         <v>18</v>
       </c>
-      <c r="B24" s="44"/>
+      <c r="B24" s="28"/>
       <c r="C24" s="14"/>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
@@ -1578,7 +1585,7 @@
       <c r="A25" s="5">
         <v>19</v>
       </c>
-      <c r="B25" s="44"/>
+      <c r="B25" s="28"/>
       <c r="C25" s="14"/>
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>
@@ -1593,7 +1600,7 @@
       <c r="A26" s="5">
         <v>20</v>
       </c>
-      <c r="B26" s="44"/>
+      <c r="B26" s="28"/>
       <c r="C26" s="14"/>
       <c r="D26" s="21"/>
       <c r="E26" s="21"/>
@@ -1608,7 +1615,7 @@
       <c r="A27" s="5">
         <v>21</v>
       </c>
-      <c r="B27" s="44"/>
+      <c r="B27" s="28"/>
       <c r="C27" s="14"/>
       <c r="D27" s="21"/>
       <c r="E27" s="21"/>
@@ -1623,7 +1630,7 @@
       <c r="A28" s="5">
         <v>22</v>
       </c>
-      <c r="B28" s="44"/>
+      <c r="B28" s="28"/>
       <c r="C28" s="14"/>
       <c r="D28" s="21"/>
       <c r="E28" s="21"/>
@@ -1638,7 +1645,7 @@
       <c r="A29" s="5">
         <v>23</v>
       </c>
-      <c r="B29" s="44"/>
+      <c r="B29" s="28"/>
       <c r="C29" s="14"/>
       <c r="D29" s="21"/>
       <c r="E29" s="21"/>
@@ -1653,7 +1660,7 @@
       <c r="A30" s="5">
         <v>24</v>
       </c>
-      <c r="B30" s="44"/>
+      <c r="B30" s="28"/>
       <c r="C30" s="14"/>
       <c r="D30" s="21"/>
       <c r="E30" s="21"/>
@@ -1668,7 +1675,7 @@
       <c r="A31" s="5">
         <v>25</v>
       </c>
-      <c r="B31" s="44"/>
+      <c r="B31" s="28"/>
       <c r="C31" s="14"/>
       <c r="D31" s="21"/>
       <c r="E31" s="21"/>
@@ -1683,7 +1690,7 @@
       <c r="A32" s="7">
         <v>26</v>
       </c>
-      <c r="B32" s="45"/>
+      <c r="B32" s="29"/>
       <c r="C32" s="15"/>
       <c r="D32" s="22"/>
       <c r="E32" s="22"/>
@@ -1716,7 +1723,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1732,58 +1739,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="27"/>
+      <c r="B3" s="31"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="31" t="s">
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="28" t="s">
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="36" t="s">
+      <c r="K5" s="40" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="33"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="35"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="39"/>
       <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1802,14 +1809,14 @@
       <c r="I6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="29"/>
-      <c r="K6" s="37"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="41"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>1</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="28" t="s">
         <v>38</v>
       </c>
       <c r="C7" s="14" t="s">
@@ -1842,7 +1849,7 @@
       <c r="A8" s="5">
         <v>2</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="28" t="s">
         <v>38</v>
       </c>
       <c r="C8" s="14" t="s">
@@ -1875,7 +1882,7 @@
       <c r="A9" s="5">
         <v>3</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="28" t="s">
         <v>38</v>
       </c>
       <c r="C9" s="14" t="s">
@@ -1908,7 +1915,7 @@
       <c r="A10" s="5">
         <v>4</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="28" t="s">
         <v>38</v>
       </c>
       <c r="C10" s="14" t="s">
@@ -1941,7 +1948,7 @@
       <c r="A11" s="5">
         <v>5</v>
       </c>
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="28" t="s">
         <v>39</v>
       </c>
       <c r="C11" s="14" t="s">
@@ -1974,7 +1981,7 @@
       <c r="A12" s="5">
         <v>6</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="28" t="s">
         <v>39</v>
       </c>
       <c r="C12" s="14" t="s">
@@ -2007,11 +2014,11 @@
       <c r="A13" s="5">
         <v>7</v>
       </c>
-      <c r="B13" s="44" t="s">
+      <c r="B13" s="28" t="s">
         <v>39</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D13" s="21" t="s">
         <v>17</v>
@@ -2023,7 +2030,7 @@
         <v>41</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H13" s="11" t="s">
         <v>41</v>
@@ -2040,11 +2047,11 @@
       <c r="A14" s="5">
         <v>8</v>
       </c>
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="28" t="s">
         <v>39</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D14" s="21" t="s">
         <v>17</v>
@@ -2056,7 +2063,7 @@
         <v>41</v>
       </c>
       <c r="G14" s="11" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H14" s="11" t="s">
         <v>41</v>
@@ -2073,8 +2080,10 @@
       <c r="A15" s="5">
         <v>9</v>
       </c>
-      <c r="B15" s="44"/>
-      <c r="C15" s="14"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="14" t="s">
+        <v>51</v>
+      </c>
       <c r="D15" s="21"/>
       <c r="E15" s="21"/>
       <c r="F15" s="21"/>
@@ -2088,8 +2097,10 @@
       <c r="A16" s="5">
         <v>10</v>
       </c>
-      <c r="B16" s="44"/>
-      <c r="C16" s="14"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="14" t="s">
+        <v>50</v>
+      </c>
       <c r="D16" s="21"/>
       <c r="E16" s="21"/>
       <c r="F16" s="21"/>
@@ -2103,7 +2114,7 @@
       <c r="A17" s="5">
         <v>11</v>
       </c>
-      <c r="B17" s="44"/>
+      <c r="B17" s="28"/>
       <c r="C17" s="14"/>
       <c r="D17" s="21"/>
       <c r="E17" s="21"/>
@@ -2118,7 +2129,7 @@
       <c r="A18" s="5">
         <v>12</v>
       </c>
-      <c r="B18" s="44"/>
+      <c r="B18" s="28"/>
       <c r="C18" s="14"/>
       <c r="D18" s="21"/>
       <c r="E18" s="21"/>
@@ -2133,7 +2144,7 @@
       <c r="A19" s="5">
         <v>13</v>
       </c>
-      <c r="B19" s="44"/>
+      <c r="B19" s="28"/>
       <c r="C19" s="14"/>
       <c r="D19" s="21"/>
       <c r="E19" s="21"/>
@@ -2148,7 +2159,7 @@
       <c r="A20" s="5">
         <v>14</v>
       </c>
-      <c r="B20" s="44"/>
+      <c r="B20" s="28"/>
       <c r="C20" s="14"/>
       <c r="D20" s="21"/>
       <c r="E20" s="21"/>
@@ -2163,7 +2174,7 @@
       <c r="A21" s="5">
         <v>15</v>
       </c>
-      <c r="B21" s="44"/>
+      <c r="B21" s="28"/>
       <c r="C21" s="14"/>
       <c r="D21" s="21"/>
       <c r="E21" s="21"/>
@@ -2178,7 +2189,7 @@
       <c r="A22" s="5">
         <v>16</v>
       </c>
-      <c r="B22" s="44"/>
+      <c r="B22" s="28"/>
       <c r="C22" s="14"/>
       <c r="D22" s="21"/>
       <c r="E22" s="21"/>
@@ -2193,7 +2204,7 @@
       <c r="A23" s="5">
         <v>17</v>
       </c>
-      <c r="B23" s="44"/>
+      <c r="B23" s="28"/>
       <c r="C23" s="14"/>
       <c r="D23" s="21"/>
       <c r="E23" s="21"/>
@@ -2208,7 +2219,7 @@
       <c r="A24" s="5">
         <v>18</v>
       </c>
-      <c r="B24" s="44"/>
+      <c r="B24" s="28"/>
       <c r="C24" s="14"/>
       <c r="D24" s="21"/>
       <c r="E24" s="21"/>
@@ -2223,7 +2234,7 @@
       <c r="A25" s="5">
         <v>19</v>
       </c>
-      <c r="B25" s="44"/>
+      <c r="B25" s="28"/>
       <c r="C25" s="14"/>
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>
@@ -2238,7 +2249,7 @@
       <c r="A26" s="5">
         <v>20</v>
       </c>
-      <c r="B26" s="44"/>
+      <c r="B26" s="28"/>
       <c r="C26" s="14"/>
       <c r="D26" s="21"/>
       <c r="E26" s="21"/>
@@ -2253,7 +2264,7 @@
       <c r="A27" s="5">
         <v>21</v>
       </c>
-      <c r="B27" s="44"/>
+      <c r="B27" s="28"/>
       <c r="C27" s="14"/>
       <c r="D27" s="21"/>
       <c r="E27" s="21"/>
@@ -2268,7 +2279,7 @@
       <c r="A28" s="5">
         <v>22</v>
       </c>
-      <c r="B28" s="44"/>
+      <c r="B28" s="28"/>
       <c r="C28" s="14"/>
       <c r="D28" s="21"/>
       <c r="E28" s="21"/>
@@ -2283,7 +2294,7 @@
       <c r="A29" s="5">
         <v>23</v>
       </c>
-      <c r="B29" s="44"/>
+      <c r="B29" s="28"/>
       <c r="C29" s="14"/>
       <c r="D29" s="21"/>
       <c r="E29" s="21"/>
@@ -2298,7 +2309,7 @@
       <c r="A30" s="5">
         <v>24</v>
       </c>
-      <c r="B30" s="44"/>
+      <c r="B30" s="28"/>
       <c r="C30" s="14"/>
       <c r="D30" s="21"/>
       <c r="E30" s="21"/>
@@ -2313,7 +2324,7 @@
       <c r="A31" s="5">
         <v>25</v>
       </c>
-      <c r="B31" s="44"/>
+      <c r="B31" s="28"/>
       <c r="C31" s="14"/>
       <c r="D31" s="21"/>
       <c r="E31" s="21"/>
@@ -2328,7 +2339,7 @@
       <c r="A32" s="7">
         <v>26</v>
       </c>
-      <c r="B32" s="45"/>
+      <c r="B32" s="29"/>
       <c r="C32" s="15"/>
       <c r="D32" s="22"/>
       <c r="E32" s="22"/>

</xml_diff>

<commit_message>
add code for BookShelf
</commit_message>
<xml_diff>
--- a/Task.xlsx
+++ b/Task.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="54">
   <si>
     <t>Num.</t>
   </si>
@@ -181,6 +181,12 @@
   </si>
   <si>
     <t>BookShelf</t>
+  </si>
+  <si>
+    <t>bookstore</t>
+  </si>
+  <si>
+    <t>3/5</t>
   </si>
 </sst>
 </file>
@@ -623,7 +629,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -649,18 +655,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -682,21 +676,12 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="10" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -710,6 +695,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -760,7 +748,19 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1074,7 +1074,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,108 +1090,108 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="31"/>
+      <c r="B3" s="25"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="35" t="s">
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="32" t="s">
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="40" t="s">
+      <c r="K5" s="34" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="43"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="25" t="s">
+      <c r="A6" s="37"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="25" t="s">
+      <c r="H6" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="I6" s="25" t="s">
+      <c r="I6" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="33"/>
-      <c r="K6" s="41"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="35"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="26">
+      <c r="A7" s="19">
         <v>1</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="24" t="s">
+      <c r="H7" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="24" t="s">
+      <c r="I7" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="J7" s="16" t="s">
+      <c r="J7" s="12" t="s">
         <v>14</v>
       </c>
       <c r="K7" s="4"/>
@@ -1200,31 +1200,31 @@
       <c r="A8" s="5">
         <v>2</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I8" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="J8" s="17" t="s">
+      <c r="J8" s="13" t="s">
         <v>14</v>
       </c>
       <c r="K8" s="6"/>
@@ -1233,31 +1233,31 @@
       <c r="A9" s="5">
         <v>3</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="20" t="s">
+      <c r="F9" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="I9" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="J9" s="17" t="s">
+      <c r="J9" s="13" t="s">
         <v>14</v>
       </c>
       <c r="K9" s="6"/>
@@ -1266,31 +1266,31 @@
       <c r="A10" s="5">
         <v>4</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="J10" s="17" t="s">
+      <c r="J10" s="13" t="s">
         <v>14</v>
       </c>
       <c r="K10" s="6"/>
@@ -1299,31 +1299,31 @@
       <c r="A11" s="5">
         <v>5</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="I11" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="J11" s="17" t="s">
+      <c r="J11" s="13" t="s">
         <v>14</v>
       </c>
       <c r="K11" s="6"/>
@@ -1332,29 +1332,29 @@
       <c r="A12" s="5">
         <v>6</v>
       </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="14" t="s">
+      <c r="B12" s="21"/>
+      <c r="C12" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="F12" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="I12" s="11" t="s">
+      <c r="I12" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="J12" s="17" t="s">
+      <c r="J12" s="13" t="s">
         <v>14</v>
       </c>
       <c r="K12" s="6" t="s">
@@ -1365,31 +1365,31 @@
       <c r="A13" s="5">
         <v>7</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="F13" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="I13" s="11" t="s">
+      <c r="I13" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="J13" s="17" t="s">
+      <c r="J13" s="13" t="s">
         <v>14</v>
       </c>
       <c r="K13" s="6"/>
@@ -1398,31 +1398,31 @@
       <c r="A14" s="5">
         <v>8</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D14" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="I14" s="46" t="s">
+      <c r="I14" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="J14" s="17" t="s">
+      <c r="J14" s="13" t="s">
         <v>14</v>
       </c>
       <c r="K14" s="6"/>
@@ -1431,274 +1431,296 @@
       <c r="A15" s="5">
         <v>9</v>
       </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="14" t="s">
+      <c r="B15" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="17"/>
+      <c r="D15" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="J15" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="K15" s="6"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>10</v>
       </c>
-      <c r="B16" s="28"/>
-      <c r="C16" s="14" t="s">
+      <c r="B16" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="17"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="13"/>
       <c r="K16" s="6"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>11</v>
       </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="17"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="13"/>
       <c r="K17" s="6"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>12</v>
       </c>
-      <c r="B18" s="28"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="17"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="13"/>
       <c r="K18" s="6"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>13</v>
       </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="17"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="13"/>
       <c r="K19" s="6"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>14</v>
       </c>
-      <c r="B20" s="28"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="17"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="13"/>
       <c r="K20" s="6"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>15</v>
       </c>
-      <c r="B21" s="28"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="17"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="13"/>
       <c r="K21" s="6"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>16</v>
       </c>
-      <c r="B22" s="28"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="17"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="13"/>
       <c r="K22" s="6"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>17</v>
       </c>
-      <c r="B23" s="28"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="17"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="13"/>
       <c r="K23" s="6"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>18</v>
       </c>
-      <c r="B24" s="28"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="17"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="13"/>
       <c r="K24" s="6"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>19</v>
       </c>
-      <c r="B25" s="28"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="17"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="13"/>
       <c r="K25" s="6"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>20</v>
       </c>
-      <c r="B26" s="28"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="17"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="13"/>
       <c r="K26" s="6"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>21</v>
       </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="17"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="13"/>
       <c r="K27" s="6"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>22</v>
       </c>
-      <c r="B28" s="28"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="17"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="13"/>
       <c r="K28" s="6"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>23</v>
       </c>
-      <c r="B29" s="28"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="17"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="13"/>
       <c r="K29" s="6"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>24</v>
       </c>
-      <c r="B30" s="28"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="17"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="13"/>
       <c r="K30" s="6"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>25</v>
       </c>
-      <c r="B31" s="28"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="17"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="13"/>
       <c r="K31" s="6"/>
     </row>
     <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7">
         <v>26</v>
       </c>
-      <c r="B32" s="29"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="12"/>
-      <c r="J32" s="18"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="14"/>
       <c r="K32" s="8"/>
     </row>
   </sheetData>
@@ -1723,7 +1745,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1739,58 +1761,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="31"/>
+      <c r="B3" s="25"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="35" t="s">
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="32" t="s">
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="40" t="s">
+      <c r="K5" s="34" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="45"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="39"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="33"/>
       <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1809,38 +1831,38 @@
       <c r="I6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="33"/>
-      <c r="K6" s="41"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="35"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>1</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="16" t="s">
+      <c r="J7" s="12" t="s">
         <v>14</v>
       </c>
       <c r="K7" s="4"/>
@@ -1849,31 +1871,31 @@
       <c r="A8" s="5">
         <v>2</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I8" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="J8" s="17" t="s">
+      <c r="J8" s="13" t="s">
         <v>14</v>
       </c>
       <c r="K8" s="6"/>
@@ -1882,31 +1904,31 @@
       <c r="A9" s="5">
         <v>3</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="20" t="s">
+      <c r="F9" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="G9" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="I9" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="J9" s="17" t="s">
+      <c r="J9" s="13" t="s">
         <v>14</v>
       </c>
       <c r="K9" s="6"/>
@@ -1915,31 +1937,31 @@
       <c r="A10" s="5">
         <v>4</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="11" t="s">
+      <c r="I10" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="J10" s="17" t="s">
+      <c r="J10" s="13" t="s">
         <v>14</v>
       </c>
       <c r="K10" s="6"/>
@@ -1948,31 +1970,31 @@
       <c r="A11" s="5">
         <v>5</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="I11" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="J11" s="17" t="s">
+      <c r="J11" s="13" t="s">
         <v>14</v>
       </c>
       <c r="K11" s="6"/>
@@ -1981,31 +2003,31 @@
       <c r="A12" s="5">
         <v>6</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="F12" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="I12" s="11" t="s">
+      <c r="I12" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="J12" s="17" t="s">
+      <c r="J12" s="13" t="s">
         <v>14</v>
       </c>
       <c r="K12" s="6"/>
@@ -2014,31 +2036,31 @@
       <c r="A13" s="5">
         <v>7</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="21" t="s">
+      <c r="F13" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="I13" s="11" t="s">
+      <c r="I13" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="J13" s="17" t="s">
+      <c r="J13" s="13" t="s">
         <v>14</v>
       </c>
       <c r="K13" s="6"/>
@@ -2047,31 +2069,31 @@
       <c r="A14" s="5">
         <v>8</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D14" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="G14" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="I14" s="11" t="s">
+      <c r="I14" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="J14" s="17" t="s">
+      <c r="J14" s="13" t="s">
         <v>14</v>
       </c>
       <c r="K14" s="6"/>
@@ -2080,274 +2102,298 @@
       <c r="A15" s="5">
         <v>9</v>
       </c>
-      <c r="B15" s="28"/>
-      <c r="C15" s="14" t="s">
+      <c r="B15" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="17"/>
+      <c r="D15" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="J15" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="K15" s="6"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>10</v>
       </c>
-      <c r="B16" s="28"/>
-      <c r="C16" s="14" t="s">
+      <c r="B16" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="17"/>
+      <c r="D16" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="13"/>
       <c r="K16" s="6"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>11</v>
       </c>
-      <c r="B17" s="28"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="17"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="13"/>
       <c r="K17" s="6"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>12</v>
       </c>
-      <c r="B18" s="28"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="17"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="13"/>
       <c r="K18" s="6"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>13</v>
       </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="17"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="13"/>
       <c r="K19" s="6"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
         <v>14</v>
       </c>
-      <c r="B20" s="28"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="17"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="13"/>
       <c r="K20" s="6"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>15</v>
       </c>
-      <c r="B21" s="28"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="17"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="13"/>
       <c r="K21" s="6"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>16</v>
       </c>
-      <c r="B22" s="28"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="17"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="13"/>
       <c r="K22" s="6"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>17</v>
       </c>
-      <c r="B23" s="28"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="17"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="13"/>
       <c r="K23" s="6"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>18</v>
       </c>
-      <c r="B24" s="28"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="17"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="13"/>
       <c r="K24" s="6"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>19</v>
       </c>
-      <c r="B25" s="28"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="17"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="13"/>
       <c r="K25" s="6"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
         <v>20</v>
       </c>
-      <c r="B26" s="28"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="17"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="13"/>
       <c r="K26" s="6"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
         <v>21</v>
       </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="17"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="13"/>
       <c r="K27" s="6"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>22</v>
       </c>
-      <c r="B28" s="28"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="17"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="13"/>
       <c r="K28" s="6"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>23</v>
       </c>
-      <c r="B29" s="28"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="21"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="17"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="13"/>
       <c r="K29" s="6"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>24</v>
       </c>
-      <c r="B30" s="28"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="17"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="13"/>
       <c r="K30" s="6"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>25</v>
       </c>
-      <c r="B31" s="28"/>
-      <c r="C31" s="14"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="17"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="13"/>
       <c r="K31" s="6"/>
     </row>
     <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7">
         <v>26</v>
       </c>
-      <c r="B32" s="29"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="22"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="12"/>
-      <c r="J32" s="18"/>
+      <c r="B32" s="22"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="41"/>
+      <c r="G32" s="42"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="42"/>
+      <c r="J32" s="14"/>
       <c r="K32" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add code for UserShippingAddress
</commit_message>
<xml_diff>
--- a/Task.xlsx
+++ b/Task.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="60">
   <si>
     <t>Num.</t>
   </si>
@@ -187,6 +187,24 @@
   </si>
   <si>
     <t>3/5</t>
+  </si>
+  <si>
+    <t>4/5</t>
+  </si>
+  <si>
+    <t>3h</t>
+  </si>
+  <si>
+    <t>7/5</t>
+  </si>
+  <si>
+    <t>UserShippingAddress</t>
+  </si>
+  <si>
+    <t>8/5</t>
+  </si>
+  <si>
+    <t>list, add, update, delete, setDefault</t>
   </si>
 </sst>
 </file>
@@ -629,7 +647,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -700,6 +718,24 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -746,21 +782,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1074,7 +1095,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,58 +1111,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="25"/>
+      <c r="B3" s="31"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="29" t="s">
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="26" t="s">
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="34" t="s">
+      <c r="K5" s="40" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="37"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="33"/>
+      <c r="A6" s="43"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="39"/>
       <c r="D6" s="18" t="s">
         <v>3</v>
       </c>
@@ -1160,8 +1181,8 @@
       <c r="I6" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="27"/>
-      <c r="K6" s="35"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="41"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="19">
@@ -1176,19 +1197,19 @@
       <c r="D7" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="43" t="s">
+      <c r="E7" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="43" t="s">
+      <c r="F7" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="44" t="s">
+      <c r="G7" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="44" t="s">
+      <c r="H7" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="44" t="s">
+      <c r="I7" s="28" t="s">
         <v>16</v>
       </c>
       <c r="J7" s="12" t="s">
@@ -1209,10 +1230,10 @@
       <c r="D8" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="40" t="s">
+      <c r="E8" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="40" t="s">
+      <c r="F8" s="24" t="s">
         <v>16</v>
       </c>
       <c r="G8" s="23" t="s">
@@ -1242,10 +1263,10 @@
       <c r="D9" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="40" t="s">
+      <c r="E9" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="40" t="s">
+      <c r="F9" s="24" t="s">
         <v>6</v>
       </c>
       <c r="G9" s="23" t="s">
@@ -1275,10 +1296,10 @@
       <c r="D10" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="40" t="s">
+      <c r="E10" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="40" t="s">
+      <c r="F10" s="24" t="s">
         <v>22</v>
       </c>
       <c r="G10" s="23" t="s">
@@ -1308,10 +1329,10 @@
       <c r="D11" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="40" t="s">
+      <c r="E11" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="40" t="s">
+      <c r="F11" s="24" t="s">
         <v>31</v>
       </c>
       <c r="G11" s="23" t="s">
@@ -1339,10 +1360,10 @@
       <c r="D12" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="40" t="s">
+      <c r="E12" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="40" t="s">
+      <c r="F12" s="24" t="s">
         <v>31</v>
       </c>
       <c r="G12" s="23" t="s">
@@ -1374,10 +1395,10 @@
       <c r="D13" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="40" t="s">
+      <c r="E13" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="40" t="s">
+      <c r="F13" s="24" t="s">
         <v>35</v>
       </c>
       <c r="G13" s="23" t="s">
@@ -1407,10 +1428,10 @@
       <c r="D14" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="40" t="s">
+      <c r="E14" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="40" t="s">
+      <c r="F14" s="24" t="s">
         <v>41</v>
       </c>
       <c r="G14" s="23" t="s">
@@ -1440,10 +1461,10 @@
       <c r="D15" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E15" s="40" t="s">
+      <c r="E15" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="40" t="s">
+      <c r="F15" s="24" t="s">
         <v>49</v>
       </c>
       <c r="G15" s="23" t="s">
@@ -1470,33 +1491,63 @@
       <c r="C16" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="40" t="s">
+      <c r="D16" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F16" s="40" t="s">
+      <c r="F16" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="13"/>
+      <c r="G16" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="I16" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="J16" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="K16" s="6"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>11</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="6"/>
+      <c r="B17" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="I17" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="J17" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="K17" s="29" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
@@ -1505,8 +1556,8 @@
       <c r="B18" s="21"/>
       <c r="C18" s="10"/>
       <c r="D18" s="16"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
       <c r="G18" s="23"/>
       <c r="H18" s="23"/>
       <c r="I18" s="23"/>
@@ -1520,8 +1571,8 @@
       <c r="B19" s="21"/>
       <c r="C19" s="10"/>
       <c r="D19" s="16"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
       <c r="G19" s="23"/>
       <c r="H19" s="23"/>
       <c r="I19" s="23"/>
@@ -1535,8 +1586,8 @@
       <c r="B20" s="21"/>
       <c r="C20" s="10"/>
       <c r="D20" s="16"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
       <c r="G20" s="23"/>
       <c r="H20" s="23"/>
       <c r="I20" s="23"/>
@@ -1550,8 +1601,8 @@
       <c r="B21" s="21"/>
       <c r="C21" s="10"/>
       <c r="D21" s="16"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
       <c r="G21" s="23"/>
       <c r="H21" s="23"/>
       <c r="I21" s="23"/>
@@ -1565,8 +1616,8 @@
       <c r="B22" s="21"/>
       <c r="C22" s="10"/>
       <c r="D22" s="16"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
       <c r="G22" s="23"/>
       <c r="H22" s="23"/>
       <c r="I22" s="23"/>
@@ -1580,8 +1631,8 @@
       <c r="B23" s="21"/>
       <c r="C23" s="10"/>
       <c r="D23" s="16"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
       <c r="G23" s="23"/>
       <c r="H23" s="23"/>
       <c r="I23" s="23"/>
@@ -1595,8 +1646,8 @@
       <c r="B24" s="21"/>
       <c r="C24" s="10"/>
       <c r="D24" s="16"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
       <c r="G24" s="23"/>
       <c r="H24" s="23"/>
       <c r="I24" s="23"/>
@@ -1610,8 +1661,8 @@
       <c r="B25" s="21"/>
       <c r="C25" s="10"/>
       <c r="D25" s="16"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="40"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
       <c r="G25" s="23"/>
       <c r="H25" s="23"/>
       <c r="I25" s="23"/>
@@ -1625,8 +1676,8 @@
       <c r="B26" s="21"/>
       <c r="C26" s="10"/>
       <c r="D26" s="16"/>
-      <c r="E26" s="40"/>
-      <c r="F26" s="40"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
       <c r="G26" s="23"/>
       <c r="H26" s="23"/>
       <c r="I26" s="23"/>
@@ -1640,8 +1691,8 @@
       <c r="B27" s="21"/>
       <c r="C27" s="10"/>
       <c r="D27" s="16"/>
-      <c r="E27" s="40"/>
-      <c r="F27" s="40"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
       <c r="G27" s="23"/>
       <c r="H27" s="23"/>
       <c r="I27" s="23"/>
@@ -1655,8 +1706,8 @@
       <c r="B28" s="21"/>
       <c r="C28" s="10"/>
       <c r="D28" s="16"/>
-      <c r="E28" s="40"/>
-      <c r="F28" s="40"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
       <c r="G28" s="23"/>
       <c r="H28" s="23"/>
       <c r="I28" s="23"/>
@@ -1670,8 +1721,8 @@
       <c r="B29" s="21"/>
       <c r="C29" s="10"/>
       <c r="D29" s="16"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
       <c r="G29" s="23"/>
       <c r="H29" s="23"/>
       <c r="I29" s="23"/>
@@ -1685,8 +1736,8 @@
       <c r="B30" s="21"/>
       <c r="C30" s="10"/>
       <c r="D30" s="16"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
       <c r="G30" s="23"/>
       <c r="H30" s="23"/>
       <c r="I30" s="23"/>
@@ -1700,8 +1751,8 @@
       <c r="B31" s="21"/>
       <c r="C31" s="10"/>
       <c r="D31" s="16"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
       <c r="G31" s="23"/>
       <c r="H31" s="23"/>
       <c r="I31" s="23"/>
@@ -1715,11 +1766,11 @@
       <c r="B32" s="22"/>
       <c r="C32" s="11"/>
       <c r="D32" s="17"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="42"/>
-      <c r="H32" s="42"/>
-      <c r="I32" s="42"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
       <c r="J32" s="14"/>
       <c r="K32" s="8"/>
     </row>
@@ -1745,7 +1796,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1761,58 +1812,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="25"/>
+      <c r="B3" s="31"/>
     </row>
     <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="29" t="s">
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="26" t="s">
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="34" t="s">
+      <c r="K5" s="40" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="39"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="33"/>
+      <c r="A6" s="45"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="39"/>
       <c r="D6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1831,8 +1882,8 @@
       <c r="I6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J6" s="27"/>
-      <c r="K6" s="35"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="41"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
@@ -1847,10 +1898,10 @@
       <c r="D7" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="40" t="s">
+      <c r="E7" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="40" t="s">
+      <c r="F7" s="24" t="s">
         <v>6</v>
       </c>
       <c r="G7" s="23" t="s">
@@ -1880,10 +1931,10 @@
       <c r="D8" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="40" t="s">
+      <c r="E8" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="40" t="s">
+      <c r="F8" s="24" t="s">
         <v>20</v>
       </c>
       <c r="G8" s="23" t="s">
@@ -1913,10 +1964,10 @@
       <c r="D9" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="40" t="s">
+      <c r="E9" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="40" t="s">
+      <c r="F9" s="24" t="s">
         <v>20</v>
       </c>
       <c r="G9" s="23" t="s">
@@ -1946,10 +1997,10 @@
       <c r="D10" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="40" t="s">
+      <c r="E10" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="40" t="s">
+      <c r="F10" s="24" t="s">
         <v>22</v>
       </c>
       <c r="G10" s="23" t="s">
@@ -1979,10 +2030,10 @@
       <c r="D11" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="40" t="s">
+      <c r="E11" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="40" t="s">
+      <c r="F11" s="24" t="s">
         <v>35</v>
       </c>
       <c r="G11" s="23" t="s">
@@ -2012,10 +2063,10 @@
       <c r="D12" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="40" t="s">
+      <c r="E12" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="40" t="s">
+      <c r="F12" s="24" t="s">
         <v>35</v>
       </c>
       <c r="G12" s="23" t="s">
@@ -2045,10 +2096,10 @@
       <c r="D13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="40" t="s">
+      <c r="E13" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="40" t="s">
+      <c r="F13" s="24" t="s">
         <v>41</v>
       </c>
       <c r="G13" s="23" t="s">
@@ -2078,10 +2129,10 @@
       <c r="D14" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="40" t="s">
+      <c r="E14" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="40" t="s">
+      <c r="F14" s="24" t="s">
         <v>41</v>
       </c>
       <c r="G14" s="23" t="s">
@@ -2111,10 +2162,10 @@
       <c r="D15" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E15" s="40" t="s">
+      <c r="E15" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="40" t="s">
+      <c r="F15" s="24" t="s">
         <v>49</v>
       </c>
       <c r="G15" s="23" t="s">
@@ -2144,31 +2195,57 @@
       <c r="D16" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="40" t="s">
+      <c r="E16" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F16" s="40" t="s">
+      <c r="F16" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="13"/>
+      <c r="G16" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="I16" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="J16" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="K16" s="6"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>11</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="13"/>
+      <c r="B17" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="I17" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="J17" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="K17" s="6"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -2178,8 +2255,8 @@
       <c r="B18" s="21"/>
       <c r="C18" s="10"/>
       <c r="D18" s="16"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
       <c r="G18" s="23"/>
       <c r="H18" s="23"/>
       <c r="I18" s="23"/>
@@ -2193,8 +2270,8 @@
       <c r="B19" s="21"/>
       <c r="C19" s="10"/>
       <c r="D19" s="16"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
       <c r="G19" s="23"/>
       <c r="H19" s="23"/>
       <c r="I19" s="23"/>
@@ -2208,8 +2285,8 @@
       <c r="B20" s="21"/>
       <c r="C20" s="10"/>
       <c r="D20" s="16"/>
-      <c r="E20" s="40"/>
-      <c r="F20" s="40"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
       <c r="G20" s="23"/>
       <c r="H20" s="23"/>
       <c r="I20" s="23"/>
@@ -2223,8 +2300,8 @@
       <c r="B21" s="21"/>
       <c r="C21" s="10"/>
       <c r="D21" s="16"/>
-      <c r="E21" s="40"/>
-      <c r="F21" s="40"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
       <c r="G21" s="23"/>
       <c r="H21" s="23"/>
       <c r="I21" s="23"/>
@@ -2238,8 +2315,8 @@
       <c r="B22" s="21"/>
       <c r="C22" s="10"/>
       <c r="D22" s="16"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
       <c r="G22" s="23"/>
       <c r="H22" s="23"/>
       <c r="I22" s="23"/>
@@ -2253,8 +2330,8 @@
       <c r="B23" s="21"/>
       <c r="C23" s="10"/>
       <c r="D23" s="16"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
       <c r="G23" s="23"/>
       <c r="H23" s="23"/>
       <c r="I23" s="23"/>
@@ -2268,8 +2345,8 @@
       <c r="B24" s="21"/>
       <c r="C24" s="10"/>
       <c r="D24" s="16"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
       <c r="G24" s="23"/>
       <c r="H24" s="23"/>
       <c r="I24" s="23"/>
@@ -2283,8 +2360,8 @@
       <c r="B25" s="21"/>
       <c r="C25" s="10"/>
       <c r="D25" s="16"/>
-      <c r="E25" s="40"/>
-      <c r="F25" s="40"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
       <c r="G25" s="23"/>
       <c r="H25" s="23"/>
       <c r="I25" s="23"/>
@@ -2298,8 +2375,8 @@
       <c r="B26" s="21"/>
       <c r="C26" s="10"/>
       <c r="D26" s="16"/>
-      <c r="E26" s="40"/>
-      <c r="F26" s="40"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
       <c r="G26" s="23"/>
       <c r="H26" s="23"/>
       <c r="I26" s="23"/>
@@ -2313,8 +2390,8 @@
       <c r="B27" s="21"/>
       <c r="C27" s="10"/>
       <c r="D27" s="16"/>
-      <c r="E27" s="40"/>
-      <c r="F27" s="40"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
       <c r="G27" s="23"/>
       <c r="H27" s="23"/>
       <c r="I27" s="23"/>
@@ -2328,8 +2405,8 @@
       <c r="B28" s="21"/>
       <c r="C28" s="10"/>
       <c r="D28" s="16"/>
-      <c r="E28" s="40"/>
-      <c r="F28" s="40"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
       <c r="G28" s="23"/>
       <c r="H28" s="23"/>
       <c r="I28" s="23"/>
@@ -2343,8 +2420,8 @@
       <c r="B29" s="21"/>
       <c r="C29" s="10"/>
       <c r="D29" s="16"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
       <c r="G29" s="23"/>
       <c r="H29" s="23"/>
       <c r="I29" s="23"/>
@@ -2358,8 +2435,8 @@
       <c r="B30" s="21"/>
       <c r="C30" s="10"/>
       <c r="D30" s="16"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
       <c r="G30" s="23"/>
       <c r="H30" s="23"/>
       <c r="I30" s="23"/>
@@ -2373,8 +2450,8 @@
       <c r="B31" s="21"/>
       <c r="C31" s="10"/>
       <c r="D31" s="16"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
       <c r="G31" s="23"/>
       <c r="H31" s="23"/>
       <c r="I31" s="23"/>
@@ -2388,11 +2465,11 @@
       <c r="B32" s="22"/>
       <c r="C32" s="11"/>
       <c r="D32" s="17"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="42"/>
-      <c r="H32" s="42"/>
-      <c r="I32" s="42"/>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
       <c r="J32" s="14"/>
       <c r="K32" s="8"/>
     </row>

</xml_diff>